<commit_message>
arrumei titulo da variavel exp_type para exp_type_manual
</commit_message>
<xml_diff>
--- a/papers experiementais.xlsx
+++ b/papers experiementais.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/66dbe330cb88da91/Doutorado/Tese/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/66dbe330cb88da91/Doutorado/TeseDoutorado/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="333" documentId="11_B89231273C296AD7B8A43B9EA75E1C27FA9FEC10" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB64F8C4-F0F7-43D1-B814-C66EA298610A}"/>
+  <xr:revisionPtr revIDLastSave="336" documentId="11_B89231273C296AD7B8A43B9EA75E1C27FA9FEC10" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B357A8A-6EE3-4A30-8824-C52377A89DFE}"/>
   <bookViews>
-    <workbookView xWindow="7185" yWindow="2595" windowWidth="19230" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -2561,9 +2561,6 @@
     <t>Laboratory</t>
   </si>
   <si>
-    <t>exp_type</t>
-  </si>
-  <si>
     <t>Laboratory; Survey</t>
   </si>
   <si>
@@ -2580,6 +2577,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>exp_type_manual</t>
   </si>
 </sst>
 </file>
@@ -2643,13 +2643,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0CAA841E-6FF1-4526-A9DB-537819374BAA}" name="Tabela2" displayName="Tabela2" ref="A1:H208" totalsRowShown="0">
-  <autoFilter ref="A1:H208" xr:uid="{0CAA841E-6FF1-4526-A9DB-537819374BAA}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="WHY CORPORATE POLITICAL CONNECTIONS CAN IMPEDE INVESTMENT"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{C46AF56D-A99F-40F5-8AE3-8E9D3AFDA073}" name="CODE"/>
     <tableColumn id="2" xr3:uid="{F8C4CBCE-4270-41E9-9B0D-4F49C0556FBC}" name="AU"/>
@@ -2658,7 +2651,7 @@
     <tableColumn id="5" xr3:uid="{0EFC5A22-9578-4F78-9F82-F0BD44A7D162}" name="SO"/>
     <tableColumn id="6" xr3:uid="{E237E8E3-D8F3-4030-ACDC-AC76CCD46DF1}" name="DI"/>
     <tableColumn id="7" xr3:uid="{3E3A815B-C7E6-4AEC-9513-67A4BE96D5B9}" name="email"/>
-    <tableColumn id="9" xr3:uid="{46886570-5239-4AC0-9DD3-6D138C7E3C16}" name="exp_type"/>
+    <tableColumn id="9" xr3:uid="{46886570-5239-4AC0-9DD3-6D138C7E3C16}" name="exp_type_manual"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2946,7 +2939,7 @@
   <dimension ref="A1:H208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2981,10 +2974,10 @@
         <v>834</v>
       </c>
       <c r="H1" t="s">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3007,7 +3000,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3030,7 +3023,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -3053,7 +3046,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -3076,7 +3069,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -3099,7 +3092,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -3122,7 +3115,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -3145,7 +3138,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -3168,7 +3161,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -3191,7 +3184,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -3214,7 +3207,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -3234,7 +3227,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -3257,10 +3250,10 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -3283,7 +3276,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -3306,7 +3299,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -3329,7 +3322,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -3352,7 +3345,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -3375,10 +3368,10 @@
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -3401,7 +3394,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -3421,7 +3414,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -3444,7 +3437,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>90</v>
       </c>
@@ -3490,7 +3483,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -3513,7 +3506,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>102</v>
       </c>
@@ -3536,7 +3529,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>106</v>
       </c>
@@ -3559,7 +3552,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>110</v>
       </c>
@@ -3582,7 +3575,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>114</v>
       </c>
@@ -3605,7 +3598,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>118</v>
       </c>
@@ -3628,7 +3621,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>122</v>
       </c>
@@ -3651,7 +3644,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>126</v>
       </c>
@@ -3674,7 +3667,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>130</v>
       </c>
@@ -3697,7 +3690,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>134</v>
       </c>
@@ -3720,7 +3713,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>138</v>
       </c>
@@ -3743,7 +3736,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>142</v>
       </c>
@@ -3766,7 +3759,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>146</v>
       </c>
@@ -3786,10 +3779,10 @@
         <v>149</v>
       </c>
       <c r="H36" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>150</v>
       </c>
@@ -3812,7 +3805,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>154</v>
       </c>
@@ -3835,7 +3828,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>158</v>
       </c>
@@ -3858,7 +3851,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>162</v>
       </c>
@@ -3881,7 +3874,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>166</v>
       </c>
@@ -3904,7 +3897,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>170</v>
       </c>
@@ -3927,7 +3920,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>174</v>
       </c>
@@ -3950,7 +3943,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>178</v>
       </c>
@@ -3973,7 +3966,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>182</v>
       </c>
@@ -3996,10 +3989,10 @@
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>186</v>
       </c>
@@ -4022,7 +4015,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>190</v>
       </c>
@@ -4045,7 +4038,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>194</v>
       </c>
@@ -4068,7 +4061,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>198</v>
       </c>
@@ -4091,7 +4084,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>202</v>
       </c>
@@ -4114,7 +4107,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>206</v>
       </c>
@@ -4137,7 +4130,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>210</v>
       </c>
@@ -4160,7 +4153,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>214</v>
       </c>
@@ -4183,7 +4176,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>218</v>
       </c>
@@ -4206,7 +4199,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>222</v>
       </c>
@@ -4229,7 +4222,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>226</v>
       </c>
@@ -4252,7 +4245,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>230</v>
       </c>
@@ -4275,7 +4268,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>234</v>
       </c>
@@ -4298,7 +4291,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>238</v>
       </c>
@@ -4321,10 +4314,10 @@
         <v>1</v>
       </c>
       <c r="H59" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>242</v>
       </c>
@@ -4347,7 +4340,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>246</v>
       </c>
@@ -4370,7 +4363,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>250</v>
       </c>
@@ -4393,7 +4386,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>254</v>
       </c>
@@ -4416,7 +4409,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>258</v>
       </c>
@@ -4439,7 +4432,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>262</v>
       </c>
@@ -4462,7 +4455,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>266</v>
       </c>
@@ -4485,10 +4478,10 @@
         <v>1</v>
       </c>
       <c r="H66" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>270</v>
       </c>
@@ -4511,7 +4504,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>274</v>
       </c>
@@ -4531,10 +4524,10 @@
         <v>277</v>
       </c>
       <c r="H68" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>278</v>
       </c>
@@ -4557,7 +4550,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>282</v>
       </c>
@@ -4580,7 +4573,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>286</v>
       </c>
@@ -4603,7 +4596,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>290</v>
       </c>
@@ -4626,7 +4619,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>294</v>
       </c>
@@ -4646,10 +4639,10 @@
         <v>297</v>
       </c>
       <c r="H73" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>298</v>
       </c>
@@ -4672,7 +4665,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>302</v>
       </c>
@@ -4695,7 +4688,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>306</v>
       </c>
@@ -4718,7 +4711,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>310</v>
       </c>
@@ -4741,7 +4734,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>314</v>
       </c>
@@ -4764,7 +4757,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>318</v>
       </c>
@@ -4787,7 +4780,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>322</v>
       </c>
@@ -4810,7 +4803,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>326</v>
       </c>
@@ -4833,7 +4826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>330</v>
       </c>
@@ -4856,7 +4849,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>334</v>
       </c>
@@ -4879,7 +4872,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>338</v>
       </c>
@@ -4899,10 +4892,10 @@
         <v>341</v>
       </c>
       <c r="H84" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>342</v>
       </c>
@@ -4925,7 +4918,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>346</v>
       </c>
@@ -4948,7 +4941,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>350</v>
       </c>
@@ -4971,7 +4964,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>354</v>
       </c>
@@ -4994,7 +4987,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>358</v>
       </c>
@@ -5017,7 +5010,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>362</v>
       </c>
@@ -5040,7 +5033,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>366</v>
       </c>
@@ -5063,7 +5056,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>370</v>
       </c>
@@ -5086,7 +5079,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>374</v>
       </c>
@@ -5109,7 +5102,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>378</v>
       </c>
@@ -5132,7 +5125,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>382</v>
       </c>
@@ -5155,7 +5148,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>386</v>
       </c>
@@ -5178,7 +5171,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>390</v>
       </c>
@@ -5201,7 +5194,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>394</v>
       </c>
@@ -5224,7 +5217,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>398</v>
       </c>
@@ -5247,7 +5240,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>402</v>
       </c>
@@ -5270,7 +5263,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>406</v>
       </c>
@@ -5293,7 +5286,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>410</v>
       </c>
@@ -5316,7 +5309,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>414</v>
       </c>
@@ -5339,7 +5332,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>418</v>
       </c>
@@ -5359,10 +5352,10 @@
         <v>421</v>
       </c>
       <c r="H104" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>422</v>
       </c>
@@ -5382,10 +5375,10 @@
         <v>425</v>
       </c>
       <c r="H105" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>426</v>
       </c>
@@ -5408,7 +5401,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>431</v>
       </c>
@@ -5431,7 +5424,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>435</v>
       </c>
@@ -5454,7 +5447,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>439</v>
       </c>
@@ -5477,7 +5470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>443</v>
       </c>
@@ -5500,7 +5493,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>447</v>
       </c>
@@ -5523,7 +5516,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>451</v>
       </c>
@@ -5546,7 +5539,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>455</v>
       </c>
@@ -5569,7 +5562,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>459</v>
       </c>
@@ -5592,7 +5585,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>463</v>
       </c>
@@ -5615,7 +5608,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>467</v>
       </c>
@@ -5638,7 +5631,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>471</v>
       </c>
@@ -5661,7 +5654,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>475</v>
       </c>
@@ -5684,7 +5677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>479</v>
       </c>
@@ -5707,7 +5700,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>483</v>
       </c>
@@ -5730,7 +5723,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>487</v>
       </c>
@@ -5753,7 +5746,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>491</v>
       </c>
@@ -5776,7 +5769,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>495</v>
       </c>
@@ -5799,7 +5792,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>499</v>
       </c>
@@ -5822,7 +5815,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>503</v>
       </c>
@@ -5845,7 +5838,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>507</v>
       </c>
@@ -5868,7 +5861,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>511</v>
       </c>
@@ -5891,7 +5884,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>515</v>
       </c>
@@ -5914,7 +5907,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>519</v>
       </c>
@@ -5937,7 +5930,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>523</v>
       </c>
@@ -5960,7 +5953,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>527</v>
       </c>
@@ -5983,7 +5976,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>530</v>
       </c>
@@ -6006,7 +5999,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>534</v>
       </c>
@@ -6029,7 +6022,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>538</v>
       </c>
@@ -6052,7 +6045,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>542</v>
       </c>
@@ -6075,7 +6068,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>546</v>
       </c>
@@ -6098,7 +6091,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>550</v>
       </c>
@@ -6121,7 +6114,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>554</v>
       </c>
@@ -6141,7 +6134,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>557</v>
       </c>
@@ -6164,7 +6157,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>561</v>
       </c>
@@ -6187,7 +6180,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>565</v>
       </c>
@@ -6210,7 +6203,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>569</v>
       </c>
@@ -6233,7 +6226,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>573</v>
       </c>
@@ -6256,7 +6249,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>577</v>
       </c>
@@ -6279,7 +6272,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>581</v>
       </c>
@@ -6302,7 +6295,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>585</v>
       </c>
@@ -6325,10 +6318,10 @@
         <v>1</v>
       </c>
       <c r="H146" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>589</v>
       </c>
@@ -6351,7 +6344,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>593</v>
       </c>
@@ -6374,7 +6367,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>597</v>
       </c>
@@ -6397,7 +6390,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>601</v>
       </c>
@@ -6420,7 +6413,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>605</v>
       </c>
@@ -6440,10 +6433,10 @@
         <v>608</v>
       </c>
       <c r="H151" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>609</v>
       </c>
@@ -6466,7 +6459,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>613</v>
       </c>
@@ -6489,7 +6482,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>617</v>
       </c>
@@ -6512,7 +6505,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>621</v>
       </c>
@@ -6535,7 +6528,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>625</v>
       </c>
@@ -6558,7 +6551,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>629</v>
       </c>
@@ -6581,7 +6574,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>633</v>
       </c>
@@ -6604,7 +6597,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>637</v>
       </c>
@@ -6627,7 +6620,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>641</v>
       </c>
@@ -6650,7 +6643,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>645</v>
       </c>
@@ -6673,7 +6666,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>649</v>
       </c>
@@ -6696,7 +6689,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>653</v>
       </c>
@@ -6719,7 +6712,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>657</v>
       </c>
@@ -6742,7 +6735,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>661</v>
       </c>
@@ -6765,7 +6758,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>665</v>
       </c>
@@ -6788,7 +6781,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>669</v>
       </c>
@@ -6811,7 +6804,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>673</v>
       </c>
@@ -6834,7 +6827,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>677</v>
       </c>
@@ -6857,7 +6850,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>680</v>
       </c>
@@ -6880,7 +6873,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>684</v>
       </c>
@@ -6903,7 +6896,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>688</v>
       </c>
@@ -6926,7 +6919,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>692</v>
       </c>
@@ -6949,7 +6942,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>696</v>
       </c>
@@ -6972,10 +6965,10 @@
         <v>1</v>
       </c>
       <c r="H174" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>700</v>
       </c>
@@ -6998,7 +6991,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>704</v>
       </c>
@@ -7021,7 +7014,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>708</v>
       </c>
@@ -7044,7 +7037,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>712</v>
       </c>
@@ -7067,7 +7060,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>716</v>
       </c>
@@ -7090,7 +7083,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>720</v>
       </c>
@@ -7113,7 +7106,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>724</v>
       </c>
@@ -7136,7 +7129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>728</v>
       </c>
@@ -7159,7 +7152,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>731</v>
       </c>
@@ -7182,7 +7175,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>735</v>
       </c>
@@ -7205,7 +7198,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>739</v>
       </c>
@@ -7228,7 +7221,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>743</v>
       </c>
@@ -7251,7 +7244,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>747</v>
       </c>
@@ -7274,7 +7267,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>751</v>
       </c>
@@ -7297,7 +7290,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>755</v>
       </c>
@@ -7320,7 +7313,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>759</v>
       </c>
@@ -7343,7 +7336,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>762</v>
       </c>
@@ -7366,7 +7359,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>766</v>
       </c>
@@ -7389,7 +7382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>770</v>
       </c>
@@ -7412,7 +7405,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>774</v>
       </c>
@@ -7435,7 +7428,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>778</v>
       </c>
@@ -7458,7 +7451,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>782</v>
       </c>
@@ -7481,7 +7474,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>786</v>
       </c>
@@ -7504,7 +7497,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>790</v>
       </c>
@@ -7527,7 +7520,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>794</v>
       </c>
@@ -7550,7 +7543,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>798</v>
       </c>
@@ -7573,7 +7566,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>802</v>
       </c>
@@ -7596,7 +7589,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>806</v>
       </c>
@@ -7619,7 +7612,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>810</v>
       </c>
@@ -7642,7 +7635,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>814</v>
       </c>
@@ -7665,7 +7658,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>818</v>
       </c>
@@ -7688,7 +7681,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>822</v>
       </c>
@@ -7711,7 +7704,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>826</v>
       </c>
@@ -7734,7 +7727,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>830</v>
       </c>

</xml_diff>